<commit_message>
implemented DDT in test_Register file
</commit_message>
<xml_diff>
--- a/ExcelFiles/data_file.xlsx
+++ b/ExcelFiles/data_file.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PaulKP\Documents\Projects\python\selenium\SeleniumHybridFramework\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C38B40-92C4-4C4E-928B-AEAA0E1F987B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B64BA3-C9AC-461F-BD56-2A4C62748C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="975" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="975" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="FirstTestSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="RegisterTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Username</t>
   </si>
@@ -49,6 +50,60 @@
   </si>
   <si>
     <t>amotoorisamplethree@gmail.com</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>telephone</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>newsletter_yes_or_no</t>
+  </si>
+  <si>
+    <t>select_user_agreement</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>Karter</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Miligan</t>
+  </si>
+  <si>
+    <t>Karen</t>
+  </si>
+  <si>
+    <t>Moris</t>
+  </si>
+  <si>
+    <t>Tod</t>
+  </si>
+  <si>
+    <t>Haris</t>
   </si>
 </sst>
 </file>
@@ -379,7 +434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -429,4 +484,147 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5478CC5E-810E-4E90-9256-5214BA5FB634}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>1234567890</v>
+      </c>
+      <c r="D2">
+        <v>12345</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>2345678910</v>
+      </c>
+      <c r="D3">
+        <v>23456</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>3456789101</v>
+      </c>
+      <c r="D4">
+        <v>34567</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>4567891012</v>
+      </c>
+      <c r="D5">
+        <v>45678</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>5678901234</v>
+      </c>
+      <c r="D6">
+        <v>56789</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>